<commit_message>
Rerun case study with IEEEG1GV and IEEEG1TS
</commit_message>
<xml_diff>
--- a/ACTIVSg200/IL200_dyn_base.xlsx
+++ b/ACTIVSg200/IL200_dyn_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/turbinegov/ACTIVSg200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E722EC-4356-0746-9AE3-80F56C1922A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB8DCB2-6C19-F844-A7CE-1C256B03B4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="2" r:id="rId1"/>
@@ -3431,7 +3431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
@@ -13806,7 +13806,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13884,7 +13884,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -13934,7 +13934,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -13984,7 +13984,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -14034,7 +14034,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -14084,7 +14084,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -14134,7 +14134,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -14184,7 +14184,7 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -14234,7 +14234,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -14284,7 +14284,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -14334,7 +14334,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -14384,7 +14384,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -14434,7 +14434,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -14484,7 +14484,7 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -14534,7 +14534,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -14584,7 +14584,7 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -14634,7 +14634,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -14684,7 +14684,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -50655,9 +50655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -50729,7 +50729,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -50773,7 +50773,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -50817,7 +50817,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -50861,7 +50861,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -50905,7 +50905,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -50949,7 +50949,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -50993,7 +50993,7 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -51037,7 +51037,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -51081,7 +51081,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -51125,7 +51125,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -51169,7 +51169,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -51213,7 +51213,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -51257,7 +51257,7 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -51301,7 +51301,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -51345,7 +51345,7 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -51389,7 +51389,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -51433,7 +51433,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -51477,7 +51477,7 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -51521,7 +51521,7 @@
         <v>1</v>
       </c>
       <c r="H20">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -51565,7 +51565,7 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -51609,7 +51609,7 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -51653,7 +51653,7 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -51697,7 +51697,7 @@
         <v>1</v>
       </c>
       <c r="H24">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -51741,7 +51741,7 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -51785,7 +51785,7 @@
         <v>1</v>
       </c>
       <c r="H26">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -51829,7 +51829,7 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -51873,7 +51873,7 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -51917,7 +51917,7 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -51961,7 +51961,7 @@
         <v>1</v>
       </c>
       <c r="H30">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -52005,7 +52005,7 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -52049,7 +52049,7 @@
         <v>1</v>
       </c>
       <c r="H32">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I32">
         <v>1</v>
@@ -52093,7 +52093,7 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -52137,7 +52137,7 @@
         <v>1</v>
       </c>
       <c r="H34">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -52181,7 +52181,7 @@
         <v>1</v>
       </c>
       <c r="H35">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -52225,7 +52225,7 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -52269,7 +52269,7 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -52313,7 +52313,7 @@
         <v>1</v>
       </c>
       <c r="H38">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -52357,7 +52357,7 @@
         <v>1</v>
       </c>
       <c r="H39">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -52401,7 +52401,7 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -52445,7 +52445,7 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -52489,7 +52489,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -52533,7 +52533,7 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -52577,7 +52577,7 @@
         <v>1</v>
       </c>
       <c r="H44">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -52621,7 +52621,7 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -52665,7 +52665,7 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -52709,7 +52709,7 @@
         <v>1</v>
       </c>
       <c r="H47">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -52753,7 +52753,7 @@
         <v>1</v>
       </c>
       <c r="H48">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -52797,7 +52797,7 @@
         <v>1</v>
       </c>
       <c r="H49">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -52841,7 +52841,7 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I50">
         <v>1</v>

</xml_diff>